<commit_message>
Final review of system. Added evaluation and finished tutorial page
</commit_message>
<xml_diff>
--- a/evaluation/Gemini-Performance.xlsx
+++ b/evaluation/Gemini-Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atifhaiqal/Developer/Uni/2024-25/COMP3003/EasyStock-Learner/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C37E245-69B0-1F48-82B4-72C137BC027E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9C2D8B-E047-4342-BC97-EF084C1F8C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{194204F8-A0E1-2C41-BEF4-E6BBF6925CC4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" xr2:uid="{194204F8-A0E1-2C41-BEF4-E6BBF6925CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -810,7 +810,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>